<commit_message>
Fixed everything, works op now!
</commit_message>
<xml_diff>
--- a/ans/result/1401CE04.xlsx
+++ b/ans/result/1401CE04.xlsx
@@ -617,7 +617,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>No.</t>
         </is>
@@ -636,7 +636,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Marking</t>
         </is>
@@ -646,7 +646,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>-3</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="D11" s="7" t="n">
@@ -655,7 +655,7 @@
       <c r="E11" s="4" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -664,12 +664,12 @@
         <v>105</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">
         <is>
-          <t>102/140</t>
+          <t>104/140</t>
         </is>
       </c>
     </row>

</xml_diff>